<commit_message>
User data with filename fix
</commit_message>
<xml_diff>
--- a/user-data/agricultural-census/agricultural-census.xlsx
+++ b/user-data/agricultural-census/agricultural-census.xlsx
@@ -33,24 +33,57 @@
     <t xml:space="preserve">source-link</t>
   </si>
   <si>
+    <t xml:space="preserve">DZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAO Country information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-wca/wca-2010/countryinfo/en/</t>
+  </si>
+  <si>
     <t xml:space="preserve">AO</t>
   </si>
   <si>
     <t xml:space="preserve">Angola</t>
   </si>
   <si>
-    <t xml:space="preserve">Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAO Country information</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://www.fao.org/economic/ess/ess-wca/wca90-country0/en/</t>
   </si>
   <si>
+    <t xml:space="preserve">BJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botswana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics Botswana press release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cso.gov.bw/images/agri_census.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">BF</t>
   </si>
   <si>
@@ -75,28 +108,94 @@
     <t xml:space="preserve">No information</t>
   </si>
   <si>
-    <t xml:space="preserve">BJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Botswana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics Botswana press release</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cso.gov.bw/images/agri_census.pdf</t>
+    <t xml:space="preserve">CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CÃ´te d'Ivoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government press release and World Bank metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.agriculture.gouv.ci/index.php?option=com_content&amp;view=article&amp;id=455:lancement-du-recensement-des-exploitants-et-exploitations-agricoles&amp;catid=65:dernieres-actualites&amp;Itemid=90 and http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.statistics-cameroon.org/news.php?id=125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Verde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Programme for the Census of Agriculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011 (planned for 2014-15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comoros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.fao.org/fileadmin/templates/ess/ess_test_folder/World_Census_Agriculture/Country_info_2000/Keydata/Comoros_Keydata.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-capacity/countrystathome/congo-launch/en/ and http://www.fao.org/economic/ess/ess-wca/en/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Djibouti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1995</t>
   </si>
   <si>
     <t xml:space="preserve">CD</t>
@@ -108,84 +207,6 @@
     <t xml:space="preserve">1990</t>
   </si>
   <si>
-    <t xml:space="preserve">CF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Programme for the Census of Agriculture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-capacity/countrystathome/congo-launch/en/ and http://www.fao.org/economic/ess/ess-wca/en/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government press release and World Bank metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.agriculture.gouv.ci/index.php?option=com_content&amp;view=article&amp;id=455:lancement-du-recensement-des-exploitants-et-exploitations-agricoles&amp;catid=65:dernieres-actualites&amp;Itemid=90 and http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cameroon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statistics Cameroon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.statistics-cameroon.org/news.php?id=125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape Verde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Djibouti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-wca/wca-2010/countryinfo/en/</t>
-  </si>
-  <si>
     <t xml:space="preserve">EG</t>
   </si>
   <si>
@@ -201,307 +222,286 @@
     <t xml:space="preserve">http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS# and http://www.fao.org/economic/ess/ess-wca/en/</t>
   </si>
   <si>
+    <t xml:space="preserve">GQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equatorial Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eritrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No recent census</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank metadata and FAO Country Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS# and http://www.fao.org/economic/ess/ess-wca/wca90-country0/en/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea-Bissau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesotho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madagascar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malawi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mozambique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Programme for the Census of Agriculture and government press release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-wca/en/ and http://www.statistics.gov.rw/about-us/news/rwanda-national-agriculture-survey-started-november-2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Tome &amp; Principe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seychelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swaziland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Togo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uganda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008-2009</t>
+  </si>
+  <si>
     <t xml:space="preserve">EH</t>
   </si>
   <si>
     <t xml:space="preserve">Western Sahara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No recent census</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eritrea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethiopia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Bank metadata and FAO Country Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS# and http://www.fao.org/economic/ess/ess-wca/wca90-country0/en/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gambia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equatorial Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guinea-Bissau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1979</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comoros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.fao.org/fileadmin/templates/ess/ess_test_folder/World_Census_Agriculture/Country_info_2000/Keydata/Comoros_Keydata.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liberia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lesotho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Bank metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://databank.worldbank.org/data/reports.aspx?source=2&amp;type=metadata&amp;series=AG.LND.IRIG.AG.ZS#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morocco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madagascar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mauritania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mauritius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malawi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mozambique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nigeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rwanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Programme for the Census of Agriculture and government press release</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.fao.org/economic/ess/ess-wca/en/ and http://www.statistics.gov.rw/about-us/news/rwanda-national-agriculture-survey-started-november-2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seychelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sierra Leone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senegal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somalia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sao Tome &amp; Principe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swaziland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011 (planned for 2014-15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Togo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunisia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanzania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uganda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008-2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
   </si>
   <si>
     <t xml:space="preserve">ZM</t>
@@ -1020,90 +1020,90 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4"/>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
+      <c r="E7"/>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -1113,112 +1113,112 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8"/>
-      <c r="F8"/>
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -1229,128 +1229,128 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>63</v>
       </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16"/>
-      <c r="F16"/>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17"/>
-      <c r="F17"/>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -1361,16 +1361,16 @@
         <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
         <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
@@ -1381,16 +1381,16 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -1401,172 +1401,180 @@
         <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23"/>
-      <c r="F23"/>
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27"/>
-      <c r="F27"/>
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30"/>
-      <c r="F30"/>
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -1578,187 +1586,183 @@
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" t="s">
-        <v>76</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F37" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42">
@@ -1769,16 +1773,16 @@
         <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43">
@@ -1789,108 +1793,104 @@
         <v>137</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="E44" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E45"/>
       <c r="F45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" t="s">
-        <v>75</v>
-      </c>
-      <c r="F47" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
@@ -1901,16 +1901,16 @@
         <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D49" t="s">
         <v>151</v>
       </c>
       <c r="E49" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -1921,16 +1921,16 @@
         <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51">
@@ -1941,16 +1941,16 @@
         <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="E51" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52">
@@ -1961,16 +1961,16 @@
         <v>157</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="E52" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53">
@@ -1987,10 +1987,10 @@
         <v>160</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54">
@@ -2001,10 +2001,10 @@
         <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
@@ -2017,7 +2017,7 @@
         <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
         <v>165</v>
@@ -2026,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
@@ -2037,10 +2037,10 @@
         <v>167</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E56"/>
       <c r="F56"/>

</xml_diff>